<commit_message>
made changes to map using email id as names may be repetitive
</commit_message>
<xml_diff>
--- a/uploads/Phish_Report.xlsx
+++ b/uploads/Phish_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarun Akash\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9460CF1A-ED12-47B2-8EEF-CF7BD6E690D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14609AF-072E-44CF-9AA8-BD6AFFC21350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
   <si>
     <t>Employee Name</t>
   </si>
@@ -31,316 +31,319 @@
     <t>Ayaan</t>
   </si>
   <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Opened</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Clicked Link</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Zayd</t>
+  </si>
+  <si>
+    <t>Submitted Details</t>
+  </si>
+  <si>
+    <t>Neil</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>Reported</t>
+  </si>
+  <si>
+    <t>Aditya</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>Sahil</t>
+  </si>
+  <si>
+    <t>Elijah</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Nikhil</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Anaya</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Meera</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Aisha</t>
+  </si>
+  <si>
+    <t>Kiara</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Tara</t>
+  </si>
+  <si>
+    <t>Leela</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Isha</t>
+  </si>
+  <si>
+    <t>Nia</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Rhea</t>
+  </si>
+  <si>
+    <t>Sana</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Saanvi</t>
+  </si>
+  <si>
+    <t>Freya</t>
+  </si>
+  <si>
+    <t>Aanya</t>
+  </si>
+  <si>
+    <t>Arya</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Riley</t>
+  </si>
+  <si>
+    <t>Casey</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Morgan</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Quinn</t>
+  </si>
+  <si>
+    <t>Skyler</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Zephyr</t>
+  </si>
+  <si>
+    <t>Nova</t>
+  </si>
+  <si>
+    <t>Orion</t>
+  </si>
+  <si>
+    <t>Lux</t>
+  </si>
+  <si>
+    <t>Juno</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Echo</t>
+  </si>
+  <si>
+    <t>Neo</t>
+  </si>
+  <si>
+    <t>Astrid</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Tanvi</t>
+  </si>
+  <si>
+    <t>Pranav</t>
+  </si>
+  <si>
+    <t>Ishaan</t>
+  </si>
+  <si>
+    <t>Divya</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>Kavya</t>
+  </si>
+  <si>
+    <t>Anirudh</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>Harsh</t>
+  </si>
+  <si>
+    <t>Nandini</t>
+  </si>
+  <si>
+    <t>Matteo</t>
+  </si>
+  <si>
+    <t>Isla</t>
+  </si>
+  <si>
+    <t>Elio</t>
+  </si>
+  <si>
+    <t>Amélie</t>
+  </si>
+  <si>
+    <t>Sven</t>
+  </si>
+  <si>
+    <t>Bianca</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Clara</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Soren</t>
+  </si>
+  <si>
+    <t>Indigo</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Ember</t>
+  </si>
+  <si>
+    <t>Onyx</t>
+  </si>
+  <si>
+    <t>Cypress</t>
+  </si>
+  <si>
+    <t>Sol</t>
+  </si>
+  <si>
+    <t>Poet</t>
+  </si>
+  <si>
+    <t>Zenith</t>
+  </si>
+  <si>
     <t>Ignored</t>
   </si>
   <si>
-    <t>Ethan</t>
-  </si>
-  <si>
-    <t>Opened</t>
-  </si>
-  <si>
-    <t>Arjun</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Clicked Link</t>
-  </si>
-  <si>
-    <t>Rohan</t>
-  </si>
-  <si>
-    <t>Zayd</t>
-  </si>
-  <si>
-    <t>Submitted Details</t>
-  </si>
-  <si>
-    <t>Neil</t>
-  </si>
-  <si>
-    <t>Omar</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
-    <t>Leo</t>
-  </si>
-  <si>
-    <t>Karan</t>
-  </si>
-  <si>
-    <t>Reported</t>
-  </si>
-  <si>
-    <t>Aditya</t>
-  </si>
-  <si>
-    <t>Julian</t>
-  </si>
-  <si>
-    <t>Nathan</t>
-  </si>
-  <si>
-    <t>Sahil</t>
-  </si>
-  <si>
-    <t>Elijah</t>
-  </si>
-  <si>
-    <t>Raj</t>
-  </si>
-  <si>
-    <t>Marcus</t>
-  </si>
-  <si>
-    <t>Nikhil</t>
-  </si>
-  <si>
-    <t>Xavier</t>
-  </si>
-  <si>
-    <t>Anaya</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Meera</t>
-  </si>
-  <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Aisha</t>
-  </si>
-  <si>
-    <t>Kiara</t>
-  </si>
-  <si>
-    <t>Maya</t>
-  </si>
-  <si>
-    <t>Sophia</t>
-  </si>
-  <si>
-    <t>Tara</t>
-  </si>
-  <si>
-    <t>Leela</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
-    <t>Isha</t>
-  </si>
-  <si>
-    <t>Nia</t>
-  </si>
-  <si>
-    <t>Ava</t>
-  </si>
-  <si>
-    <t>Rhea</t>
-  </si>
-  <si>
-    <t>Sana</t>
-  </si>
-  <si>
-    <t>Lily</t>
-  </si>
-  <si>
-    <t>Saanvi</t>
-  </si>
-  <si>
-    <t>Freya</t>
-  </si>
-  <si>
-    <t>Aanya</t>
-  </si>
-  <si>
-    <t>Arya</t>
-  </si>
-  <si>
-    <t>Jordan</t>
-  </si>
-  <si>
-    <t>Riley</t>
-  </si>
-  <si>
-    <t>Casey</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Quinn</t>
-  </si>
-  <si>
-    <t>Skyler</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Elizabeth</t>
-  </si>
-  <si>
-    <t>Charles</t>
-  </si>
-  <si>
-    <t>Catherine</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>George</t>
-  </si>
-  <si>
-    <t>Grace</t>
-  </si>
-  <si>
-    <t>Zephyr</t>
-  </si>
-  <si>
-    <t>Nova</t>
-  </si>
-  <si>
-    <t>Orion</t>
-  </si>
-  <si>
-    <t>Lux</t>
-  </si>
-  <si>
-    <t>Juno</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>Echo</t>
-  </si>
-  <si>
-    <t>Neo</t>
-  </si>
-  <si>
-    <t>Astrid</t>
-  </si>
-  <si>
-    <t>Blaze</t>
-  </si>
-  <si>
-    <t>Tanvi</t>
-  </si>
-  <si>
-    <t>Pranav</t>
-  </si>
-  <si>
-    <t>Ishaan</t>
-  </si>
-  <si>
-    <t>Divya</t>
-  </si>
-  <si>
-    <t>Krish</t>
-  </si>
-  <si>
-    <t>Kavya</t>
-  </si>
-  <si>
-    <t>Anirudh</t>
-  </si>
-  <si>
-    <t>Sneha</t>
-  </si>
-  <si>
-    <t>Harsh</t>
-  </si>
-  <si>
-    <t>Nandini</t>
-  </si>
-  <si>
-    <t>Matteo</t>
-  </si>
-  <si>
-    <t>Isla</t>
-  </si>
-  <si>
-    <t>Elio</t>
-  </si>
-  <si>
-    <t>Amélie</t>
-  </si>
-  <si>
-    <t>Sven</t>
-  </si>
-  <si>
-    <t>Bianca</t>
-  </si>
-  <si>
-    <t>Hugo</t>
-  </si>
-  <si>
-    <t>Clara</t>
-  </si>
-  <si>
-    <t>Luca</t>
-  </si>
-  <si>
-    <t>Soren</t>
-  </si>
-  <si>
-    <t>Indigo</t>
-  </si>
-  <si>
-    <t>River</t>
-  </si>
-  <si>
-    <t>Storm</t>
-  </si>
-  <si>
-    <t>Ocean</t>
-  </si>
-  <si>
-    <t>Ember</t>
-  </si>
-  <si>
-    <t>Onyx</t>
-  </si>
-  <si>
-    <t>Cypress</t>
-  </si>
-  <si>
-    <t>Sol</t>
-  </si>
-  <si>
-    <t>Poet</t>
-  </si>
-  <si>
-    <t>Zenith</t>
+    <t>Tarun</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,15 @@
   <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -631,803 +639,808 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="2"/>
+      <c r="A102" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="2"/>

</xml_diff>